<commit_message>
Improve Previous Code with Apex Methods
</commit_message>
<xml_diff>
--- a/me/4.Apex-Classes-and-Methods.xlsx
+++ b/me/4.Apex-Classes-and-Methods.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\salesforce\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F3D048-8413-4883-8F82-84756302FABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D727CF6A-A4BA-4DDE-87BE-03A6D2E147AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apex Class" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Polymorphic Methods" sheetId="4" r:id="rId4"/>
     <sheet name="Static Keyword" sheetId="5" r:id="rId5"/>
     <sheet name="Apex Naming Conventions" sheetId="6" r:id="rId6"/>
+    <sheet name="Improve Previous Code" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="221">
   <si>
     <t>Để có overview về các tool khác nhau có thể dùng để viết code Apex trong Salesforce thì thay cho dùng developer console mình sẽ dùng Salesforce set up để tạo class</t>
   </si>
@@ -632,6 +633,108 @@
   </si>
   <si>
     <t>method: camelCase</t>
+  </si>
+  <si>
+    <t>Improve Previous Code with Apex Methods</t>
+  </si>
+  <si>
+    <t>7.improve-previous-code-with-methods</t>
+  </si>
+  <si>
+    <t>Friends.apxc</t>
+  </si>
+  <si>
+    <t>salesforce\4.Apex-Classes-and-Methods\7.improve-previous-code-with-methods\Friends.apxc</t>
+  </si>
+  <si>
+    <t>public class Friends {</t>
+  </si>
+  <si>
+    <t>/*Pizza Rates:</t>
+  </si>
+  <si>
+    <t>1 slice - $8/slice</t>
+  </si>
+  <si>
+    <t>2-3 slice - $7/slice</t>
+  </si>
+  <si>
+    <t>&gt;3 slice - $6/slice</t>
+  </si>
+  <si>
+    <t>Ross ordered - 3 slices</t>
+  </si>
+  <si>
+    <t>Chandler ordered - 1 slice</t>
+  </si>
+  <si>
+    <t>Joey ordered - 4 slices</t>
+  </si>
+  <si>
+    <t>    //Create rate card with constants</t>
+  </si>
+  <si>
+    <t>    final Integer ONLY_ONE_SLICE = 8;</t>
+  </si>
+  <si>
+    <t>    final Integer UPTO_THREE_SLICES = 7;</t>
+  </si>
+  <si>
+    <t>    final Integer MORE_THAN_THREE_SLICES = 6;</t>
+  </si>
+  <si>
+    <t>    // this method accepts number slices</t>
+  </si>
+  <si>
+    <t>    // and returns the amount</t>
+  </si>
+  <si>
+    <t>    public Integer getBill(Integer numberOfSlices){</t>
+  </si>
+  <si>
+    <t>        Integer billAmount = numberOfSlices == 1 ? ONLY_ONE_SLICE*numberOfSlices :</t>
+  </si>
+  <si>
+    <t>                            (numberOfSlices &lt;= 3 ? UPTO_THREE_SLICES*numberOfSlices :</t>
+  </si>
+  <si>
+    <t>                                MORE_THAN_THREE_SLICES*numberOfSlices);</t>
+  </si>
+  <si>
+    <t>        return billAmount;</t>
+  </si>
+  <si>
+    <t>salesforce\4.Apex-Classes-and-Methods\7.improve-previous-code-with-methods\dev-console.txt</t>
+  </si>
+  <si>
+    <t>Friends pizzaNight = new Friends();</t>
+  </si>
+  <si>
+    <t>// Calculate Ross's amount</t>
+  </si>
+  <si>
+    <t>Integer rossHasToPay = pizzaNight.getBill(3);</t>
+  </si>
+  <si>
+    <t>System.debug('Ross has to pay - '+rossHasToPay);</t>
+  </si>
+  <si>
+    <t>// Calculate Chandler's amount</t>
+  </si>
+  <si>
+    <t>Integer chandlerHasToPay = pizzaNight.getBill(1);</t>
+  </si>
+  <si>
+    <t>System.debug('Chandler has to pay - '+chandlerHasToPay);</t>
+  </si>
+  <si>
+    <t>// Calculate Joey's amount</t>
+  </si>
+  <si>
+    <t>Integer joeyHasToPay = pizzaNight.getBill(4);</t>
+  </si>
+  <si>
+    <t>System.debug('Joey has to pay - '+joeyHasToPay);</t>
   </si>
 </sst>
 </file>
@@ -2432,6 +2535,320 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>322224</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>65911</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D50CB7D0-38B7-5B08-EFD0-8A214DE05E2C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4991100" y="11858625"/>
+          <a:ext cx="13009524" cy="6114286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE539E4B-969C-FB64-4937-D52C867E5C06}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3543300" y="12687300"/>
+          <a:ext cx="4838700" cy="885825"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B2AF2DF-087F-DC7B-F2FA-68579AE60A77}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4086225" y="13468350"/>
+          <a:ext cx="4314825" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEF80877-E3BB-96E8-4D9B-D9913A0D8626}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3648075" y="14030325"/>
+          <a:ext cx="4781550" cy="104775"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1EA5B893-1F51-96DE-EA92-14B01B6CAFF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2028825" y="8915400"/>
+          <a:ext cx="1085850" cy="3533775"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39C4FC9A-44E9-EEB0-7FC2-13492A682753}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1524000" y="9144000"/>
+          <a:ext cx="1543050" cy="4810125"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -6935,8 +7352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF1060C2-2C8A-4DB7-97EC-E57109886525}">
   <dimension ref="A2:L58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I54" sqref="D54:I54"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7089,24 +7506,21 @@
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
-      <c r="D26" s="13" t="s">
+      <c r="D26" t="s">
         <v>124</v>
       </c>
-      <c r="E26" s="13"/>
       <c r="H26" s="6"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13" t="s">
+      <c r="E27" t="s">
         <v>125</v>
       </c>
       <c r="H27" s="6"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13" t="s">
+      <c r="E28" t="s">
         <v>9</v>
       </c>
       <c r="H28" s="6"/>
@@ -7157,6 +7571,426 @@
       <c r="B36" s="5" t="s">
         <v>164</v>
       </c>
+      <c r="J36" s="6"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B37" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="J37" s="6"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B38" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="J38" s="6"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B39" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="J39" s="6"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B40" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="J40" s="6"/>
+      <c r="K40" t="s">
+        <v>5</v>
+      </c>
+      <c r="L40" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B41" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="J41" s="6"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B42" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="J42" s="6"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B43" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="J43" s="6"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B44" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="J44" s="6"/>
+      <c r="K44" t="s">
+        <v>5</v>
+      </c>
+      <c r="L44" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B45" s="5"/>
+      <c r="J45" s="6"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B46" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="J46" s="6"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B47" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="J47" s="6"/>
+      <c r="K47" t="s">
+        <v>5</v>
+      </c>
+      <c r="L47" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B48" s="5"/>
+      <c r="J48" s="6"/>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B49" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="J49" s="6"/>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B50" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="J50" s="6"/>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B51" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="J51" s="6"/>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B52" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="J52" s="6"/>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B53" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="J53" s="6"/>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B54" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="J54" s="6"/>
+      <c r="K54" t="s">
+        <v>5</v>
+      </c>
+      <c r="L54" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B55" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="J55" s="6"/>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B56" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="J56" s="6"/>
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B57" s="5"/>
+      <c r="J57" s="6"/>
+    </row>
+    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B58" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="8"/>
+      <c r="I58" s="8"/>
+      <c r="J58" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB430E6B-A3DF-407F-B5F0-ECCC7C0E1F4B}">
+  <dimension ref="A2:J75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="F79" sqref="F79"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="5"/>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="5"/>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
+      <c r="D16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="D19" t="s">
+        <v>102</v>
+      </c>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="D22" t="s">
+        <v>124</v>
+      </c>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="E23" t="s">
+        <v>125</v>
+      </c>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="E24" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="D25" t="s">
+        <v>161</v>
+      </c>
+      <c r="E25" s="10"/>
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
+      <c r="E26" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="H26" s="6"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="D27" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="E27" s="10"/>
+      <c r="H27" s="6"/>
+      <c r="I27" t="s">
+        <v>5</v>
+      </c>
+      <c r="J27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="E28" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H28" s="6"/>
+      <c r="I28" t="s">
+        <v>5</v>
+      </c>
+      <c r="J28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
+      <c r="E29" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="H29" s="6"/>
+      <c r="I29" t="s">
+        <v>5</v>
+      </c>
+      <c r="J29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="7"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="9"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B34" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="4"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B35" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="6"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B36" s="5" t="s">
+        <v>193</v>
+      </c>
       <c r="C36" s="14"/>
       <c r="D36" s="14"/>
       <c r="E36" s="14"/>
@@ -7166,9 +8000,9 @@
       <c r="I36" s="14"/>
       <c r="J36" s="6"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
-        <v>165</v>
+        <v>194</v>
       </c>
       <c r="C37" s="14"/>
       <c r="D37" s="14"/>
@@ -7179,9 +8013,9 @@
       <c r="I37" s="14"/>
       <c r="J37" s="6"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
-        <v>166</v>
+        <v>195</v>
       </c>
       <c r="C38" s="14"/>
       <c r="D38" s="14"/>
@@ -7192,10 +8026,8 @@
       <c r="I38" s="14"/>
       <c r="J38" s="6"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B39" s="5" t="s">
-        <v>167</v>
-      </c>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B39" s="5"/>
       <c r="C39" s="14"/>
       <c r="D39" s="14"/>
       <c r="E39" s="14"/>
@@ -7205,9 +8037,9 @@
       <c r="I39" s="14"/>
       <c r="J39" s="6"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
-        <v>168</v>
+        <v>196</v>
       </c>
       <c r="C40" s="14"/>
       <c r="D40" s="14"/>
@@ -7217,16 +8049,10 @@
       <c r="H40" s="14"/>
       <c r="I40" s="14"/>
       <c r="J40" s="6"/>
-      <c r="K40" t="s">
-        <v>5</v>
-      </c>
-      <c r="L40" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
-        <v>169</v>
+        <v>197</v>
       </c>
       <c r="C41" s="14"/>
       <c r="D41" s="14"/>
@@ -7237,9 +8063,9 @@
       <c r="I41" s="14"/>
       <c r="J41" s="6"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
-        <v>170</v>
+        <v>198</v>
       </c>
       <c r="C42" s="14"/>
       <c r="D42" s="14"/>
@@ -7250,9 +8076,9 @@
       <c r="I42" s="14"/>
       <c r="J42" s="6"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
-        <v>171</v>
+        <v>94</v>
       </c>
       <c r="C43" s="14"/>
       <c r="D43" s="14"/>
@@ -7263,10 +8089,8 @@
       <c r="I43" s="14"/>
       <c r="J43" s="6"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B44" s="5" t="s">
-        <v>172</v>
-      </c>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B44" s="5"/>
       <c r="C44" s="14"/>
       <c r="D44" s="14"/>
       <c r="E44" s="14"/>
@@ -7275,15 +8099,11 @@
       <c r="H44" s="14"/>
       <c r="I44" s="14"/>
       <c r="J44" s="6"/>
-      <c r="K44" t="s">
-        <v>5</v>
-      </c>
-      <c r="L44" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B45" s="5"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B45" s="5" t="s">
+        <v>199</v>
+      </c>
       <c r="C45" s="14"/>
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
@@ -7293,9 +8113,9 @@
       <c r="I45" s="14"/>
       <c r="J45" s="6"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
-        <v>173</v>
+        <v>200</v>
       </c>
       <c r="C46" s="14"/>
       <c r="D46" s="14"/>
@@ -7306,9 +8126,9 @@
       <c r="I46" s="14"/>
       <c r="J46" s="6"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
-        <v>174</v>
+        <v>201</v>
       </c>
       <c r="C47" s="14"/>
       <c r="D47" s="14"/>
@@ -7318,15 +8138,11 @@
       <c r="H47" s="14"/>
       <c r="I47" s="14"/>
       <c r="J47" s="6"/>
-      <c r="K47" t="s">
-        <v>5</v>
-      </c>
-      <c r="L47" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B48" s="5"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B48" s="5" t="s">
+        <v>202</v>
+      </c>
       <c r="C48" s="14"/>
       <c r="D48" s="14"/>
       <c r="E48" s="14"/>
@@ -7336,10 +8152,8 @@
       <c r="I48" s="14"/>
       <c r="J48" s="6"/>
     </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B49" s="5" t="s">
-        <v>175</v>
-      </c>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B49" s="5"/>
       <c r="C49" s="14"/>
       <c r="D49" s="14"/>
       <c r="E49" s="14"/>
@@ -7349,9 +8163,9 @@
       <c r="I49" s="14"/>
       <c r="J49" s="6"/>
     </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
-        <v>176</v>
+        <v>203</v>
       </c>
       <c r="C50" s="14"/>
       <c r="D50" s="14"/>
@@ -7362,9 +8176,9 @@
       <c r="I50" s="14"/>
       <c r="J50" s="6"/>
     </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
-        <v>177</v>
+        <v>204</v>
       </c>
       <c r="C51" s="14"/>
       <c r="D51" s="14"/>
@@ -7375,9 +8189,9 @@
       <c r="I51" s="14"/>
       <c r="J51" s="6"/>
     </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
-        <v>178</v>
+        <v>205</v>
       </c>
       <c r="C52" s="14"/>
       <c r="D52" s="14"/>
@@ -7388,9 +8202,9 @@
       <c r="I52" s="14"/>
       <c r="J52" s="6"/>
     </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B53" s="5" t="s">
-        <v>179</v>
+        <v>206</v>
       </c>
       <c r="C53" s="14"/>
       <c r="D53" s="14"/>
@@ -7401,9 +8215,9 @@
       <c r="I53" s="14"/>
       <c r="J53" s="6"/>
     </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B54" s="5" t="s">
-        <v>180</v>
+        <v>207</v>
       </c>
       <c r="C54" s="14"/>
       <c r="D54" s="14"/>
@@ -7413,16 +8227,10 @@
       <c r="H54" s="14"/>
       <c r="I54" s="14"/>
       <c r="J54" s="6"/>
-      <c r="K54" t="s">
-        <v>5</v>
-      </c>
-      <c r="L54" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B55" s="5" t="s">
-        <v>181</v>
+        <v>208</v>
       </c>
       <c r="C55" s="14"/>
       <c r="D55" s="14"/>
@@ -7433,9 +8241,9 @@
       <c r="I55" s="14"/>
       <c r="J55" s="6"/>
     </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B56" s="5" t="s">
-        <v>182</v>
+        <v>209</v>
       </c>
       <c r="C56" s="14"/>
       <c r="D56" s="14"/>
@@ -7446,8 +8254,10 @@
       <c r="I56" s="14"/>
       <c r="J56" s="6"/>
     </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B57" s="5"/>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B57" s="5" t="s">
+        <v>182</v>
+      </c>
       <c r="C57" s="14"/>
       <c r="D57" s="14"/>
       <c r="E57" s="14"/>
@@ -7457,20 +8267,162 @@
       <c r="I57" s="14"/>
       <c r="J57" s="6"/>
     </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B58" s="7" t="s">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B58" s="5"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="14"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="14"/>
+      <c r="J58" s="6"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B59" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C58" s="8"/>
-      <c r="D58" s="8"/>
-      <c r="E58" s="8"/>
-      <c r="F58" s="8"/>
-      <c r="G58" s="8"/>
-      <c r="H58" s="8"/>
-      <c r="I58" s="8"/>
-      <c r="J58" s="9"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
+      <c r="F59" s="8"/>
+      <c r="G59" s="8"/>
+      <c r="H59" s="8"/>
+      <c r="I59" s="8"/>
+      <c r="J59" s="9"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B63" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="4"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B64" s="5"/>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="14"/>
+      <c r="F64" s="14"/>
+      <c r="G64" s="6"/>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B65" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="6"/>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B66" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="14"/>
+      <c r="G66" s="6"/>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B67" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="C67" s="14"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="14"/>
+      <c r="G67" s="6"/>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B68" s="5"/>
+      <c r="C68" s="14"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="14"/>
+      <c r="G68" s="6"/>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B69" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="C69" s="14"/>
+      <c r="D69" s="14"/>
+      <c r="E69" s="14"/>
+      <c r="F69" s="14"/>
+      <c r="G69" s="6"/>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B70" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="C70" s="14"/>
+      <c r="D70" s="14"/>
+      <c r="E70" s="14"/>
+      <c r="F70" s="14"/>
+      <c r="G70" s="6"/>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B71" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C71" s="14"/>
+      <c r="D71" s="14"/>
+      <c r="E71" s="14"/>
+      <c r="F71" s="14"/>
+      <c r="G71" s="6"/>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B72" s="5"/>
+      <c r="C72" s="14"/>
+      <c r="D72" s="14"/>
+      <c r="E72" s="14"/>
+      <c r="F72" s="14"/>
+      <c r="G72" s="6"/>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B73" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C73" s="14"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="14"/>
+      <c r="F73" s="14"/>
+      <c r="G73" s="6"/>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B74" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C74" s="14"/>
+      <c r="D74" s="14"/>
+      <c r="E74" s="14"/>
+      <c r="F74" s="14"/>
+      <c r="G74" s="6"/>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B75" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="C75" s="8"/>
+      <c r="D75" s="8"/>
+      <c r="E75" s="8"/>
+      <c r="F75" s="8"/>
+      <c r="G75" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Challenge - Apex Methods
</commit_message>
<xml_diff>
--- a/me/4.Apex-Classes-and-Methods.xlsx
+++ b/me/4.Apex-Classes-and-Methods.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\salesforce\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D727CF6A-A4BA-4DDE-87BE-03A6D2E147AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B47AF1-C144-48A4-AE20-4626AB238C64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apex Class" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Static Keyword" sheetId="5" r:id="rId5"/>
     <sheet name="Apex Naming Conventions" sheetId="6" r:id="rId6"/>
     <sheet name="Improve Previous Code" sheetId="7" r:id="rId7"/>
+    <sheet name="Challenge - Apex Methods" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="251">
   <si>
     <t>Để có overview về các tool khác nhau có thể dùng để viết code Apex trong Salesforce thì thay cho dùng developer console mình sẽ dùng Salesforce set up để tạo class</t>
   </si>
@@ -735,6 +736,96 @@
   </si>
   <si>
     <t>System.debug('Joey has to pay - '+joeyHasToPay);</t>
+  </si>
+  <si>
+    <t>8.apex-method-challenge-solution</t>
+  </si>
+  <si>
+    <t>Fitness.apxc</t>
+  </si>
+  <si>
+    <t>salesforce\4.Apex-Classes-and-Methods\8.apex-method-challenge-solution\Fitness.apxc</t>
+  </si>
+  <si>
+    <t> * Fitness class with helpful methods</t>
+  </si>
+  <si>
+    <t> * to calculate human fitness</t>
+  </si>
+  <si>
+    <t>public class Fitness {</t>
+  </si>
+  <si>
+    <t>     * calculateBMI method</t>
+  </si>
+  <si>
+    <t>     * accepts body weight (should be in kg)</t>
+  </si>
+  <si>
+    <t>     * and body height (should be in meter)</t>
+  </si>
+  <si>
+    <t>     * returns BMI value</t>
+  </si>
+  <si>
+    <t>    public static Decimal calculateBMI(Decimal weight, Decimal height) {</t>
+  </si>
+  <si>
+    <t>        Decimal result  = weight / (height*height);</t>
+  </si>
+  <si>
+    <t>        return result;</t>
+  </si>
+  <si>
+    <t>     * calculatePace method</t>
+  </si>
+  <si>
+    <t>     * accepts distance (in km)</t>
+  </si>
+  <si>
+    <t>     * and minutes</t>
+  </si>
+  <si>
+    <t>     * returns pace in km/hr</t>
+  </si>
+  <si>
+    <t>    public static Decimal calculatePace(Decimal distance, Decimal minutes) {</t>
+  </si>
+  <si>
+    <t>        Decimal hr = minutes/60;</t>
+  </si>
+  <si>
+    <t>        Decimal pace = distance / hr;</t>
+  </si>
+  <si>
+    <t>        return pace;</t>
+  </si>
+  <si>
+    <t>salesforce\4.Apex-Classes-and-Methods\8.apex-method-challenge-solution\dev-console.txt</t>
+  </si>
+  <si>
+    <t>System.debug('BMI for height '+1.2+' meter and weight '+65+'kg is : '+Fitness.calculateBMI(65, 1.2));</t>
+  </si>
+  <si>
+    <t>System.debug('BMI for height '+1.3+' meter and weight '+75+'kg is : '+Fitness.calculateBMI(75, 1.3));</t>
+  </si>
+  <si>
+    <t>System.debug('BMI for height '+1.4+' meter and weight '+87+'kg is : '+Fitness.calculateBMI(87, 1.4));</t>
+  </si>
+  <si>
+    <t>System.debug('BMI for height '+1.5+' meter and weight '+92+'kg is : '+Fitness.calculateBMI(92, 1.5));</t>
+  </si>
+  <si>
+    <t>System.debug('Pace (km/hr) for '+12.5+' km in '+80+' minutes is '+Fitness.calculatePace(12.5, 80));</t>
+  </si>
+  <si>
+    <t>System.debug('Pace (km/hr) for '+14.2+' km in '+72.3+' minutes is '+Fitness.calculatePace(14.2, 72.3));</t>
+  </si>
+  <si>
+    <t>System.debug('Pace (km/hr) for '+12.9+' km in '+60.5+' minutes is '+Fitness.calculatePace(12.9, 60.5));</t>
+  </si>
+  <si>
+    <t>System.debug('Pace (km/hr) for '+10.1+' km in '+70.1+' minutes is '+Fitness.calculatePace(10.1, 70.1));</t>
   </si>
 </sst>
 </file>
@@ -2849,6 +2940,161 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A521CC4E-34B1-973C-0732-84D092F796FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2047875" y="8896350"/>
+          <a:ext cx="3143250" cy="3762375"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4BAEB41-C214-DF89-9738-D1887D5204B4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2019300" y="11001375"/>
+          <a:ext cx="2914650" cy="2800350"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>23505</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C6E425B-E903-68B9-FACA-5B9DAA3B7810}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="695325" y="14744700"/>
+          <a:ext cx="11344275" cy="5090805"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -7739,8 +7985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB430E6B-A3DF-407F-B5F0-ECCC7C0E1F4B}">
   <dimension ref="A2:J75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="F79" sqref="F79"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7902,7 +8148,7 @@
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
-      <c r="E26" s="13" t="s">
+      <c r="E26" t="s">
         <v>162</v>
       </c>
       <c r="H26" s="6"/>
@@ -7978,304 +8224,136 @@
       <c r="B35" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
       <c r="J36" s="6"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
       <c r="J37" s="6"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
       <c r="J38" s="6"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B39" s="5"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
       <c r="J39" s="6"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
       <c r="J40" s="6"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B42" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
       <c r="J43" s="6"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B44" s="5"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
       <c r="J44" s="6"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="14"/>
       <c r="J45" s="6"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="14"/>
       <c r="J46" s="6"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="14"/>
       <c r="J47" s="6"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="14"/>
       <c r="J48" s="6"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B49" s="5"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="14"/>
       <c r="J49" s="6"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="14"/>
       <c r="J50" s="6"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
-      <c r="H51" s="14"/>
-      <c r="I51" s="14"/>
       <c r="J51" s="6"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="14"/>
       <c r="J52" s="6"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B53" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="C53" s="14"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="14"/>
-      <c r="I53" s="14"/>
       <c r="J53" s="6"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B54" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
-      <c r="H54" s="14"/>
-      <c r="I54" s="14"/>
       <c r="J54" s="6"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B55" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="C55" s="14"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="14"/>
       <c r="J55" s="6"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B56" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="C56" s="14"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14"/>
-      <c r="I56" s="14"/>
       <c r="J56" s="6"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B57" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
-      <c r="I57" s="14"/>
       <c r="J57" s="6"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B58" s="5"/>
-      <c r="C58" s="14"/>
-      <c r="D58" s="14"/>
-      <c r="E58" s="14"/>
-      <c r="F58" s="14"/>
-      <c r="G58" s="14"/>
-      <c r="H58" s="14"/>
-      <c r="I58" s="14"/>
       <c r="J58" s="6"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
@@ -8308,117 +8386,792 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B64" s="5"/>
-      <c r="C64" s="14"/>
-      <c r="D64" s="14"/>
-      <c r="E64" s="14"/>
-      <c r="F64" s="14"/>
       <c r="G64" s="6"/>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B65" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="C65" s="14"/>
-      <c r="D65" s="14"/>
-      <c r="E65" s="14"/>
-      <c r="F65" s="14"/>
       <c r="G65" s="6"/>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B66" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="C66" s="14"/>
-      <c r="D66" s="14"/>
-      <c r="E66" s="14"/>
-      <c r="F66" s="14"/>
       <c r="G66" s="6"/>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B67" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="C67" s="14"/>
-      <c r="D67" s="14"/>
-      <c r="E67" s="14"/>
-      <c r="F67" s="14"/>
       <c r="G67" s="6"/>
     </row>
     <row r="68" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B68" s="5"/>
+      <c r="G68" s="6"/>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B69" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="G69" s="6"/>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B70" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G70" s="6"/>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B71" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="G71" s="6"/>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B72" s="5"/>
+      <c r="G72" s="6"/>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B73" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="G73" s="6"/>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B74" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="G74" s="6"/>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B75" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="C75" s="8"/>
+      <c r="D75" s="8"/>
+      <c r="E75" s="8"/>
+      <c r="F75" s="8"/>
+      <c r="G75" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0489476-EE10-4190-AA21-607962102C97}">
+  <dimension ref="A3:K76"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="M75" sqref="M75"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="5"/>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="5"/>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="5"/>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="5"/>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+      <c r="D14" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="D17" t="s">
+        <v>102</v>
+      </c>
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="D20" t="s">
+        <v>124</v>
+      </c>
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="E21" t="s">
+        <v>125</v>
+      </c>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="E22" t="s">
+        <v>9</v>
+      </c>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="D23" t="s">
+        <v>161</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="E24" t="s">
+        <v>162</v>
+      </c>
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="D25" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="E25" s="13"/>
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26" s="6"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="H27" s="6"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="D28" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="E28" s="10"/>
+      <c r="H28" s="6"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
+      <c r="E29" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H29" s="6"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="5"/>
+      <c r="E30" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="H30" s="6"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="7"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="9"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="4"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="6"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="6"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="6"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="6"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="5"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="6"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="6"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B42" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="6"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="6"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="6"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="6"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
+      <c r="I46" s="6"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B47" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="6"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B48" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="6"/>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B49" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="6"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B50" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="6"/>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B51" s="5"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="6"/>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B52" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="6"/>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B53" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="6"/>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B54" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14"/>
+      <c r="I54" s="6"/>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B55" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14"/>
+      <c r="I55" s="6"/>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B56" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14"/>
+      <c r="I56" s="6"/>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B57" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="14"/>
+      <c r="H57" s="14"/>
+      <c r="I57" s="6"/>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B58" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="14"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="6"/>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B59" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="14"/>
+      <c r="H59" s="14"/>
+      <c r="I59" s="6"/>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B60" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="14"/>
+      <c r="H60" s="14"/>
+      <c r="I60" s="6"/>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B61" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
+      <c r="G61" s="14"/>
+      <c r="H61" s="14"/>
+      <c r="I61" s="6"/>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B62" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C62" s="14"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
+      <c r="G62" s="14"/>
+      <c r="H62" s="14"/>
+      <c r="I62" s="6"/>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B63" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C63" s="8"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="8"/>
+      <c r="G63" s="8"/>
+      <c r="H63" s="8"/>
+      <c r="I63" s="9"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B67" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="3"/>
+      <c r="J67" s="3"/>
+      <c r="K67" s="4"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B68" s="5" t="s">
+        <v>244</v>
+      </c>
       <c r="C68" s="14"/>
       <c r="D68" s="14"/>
       <c r="E68" s="14"/>
       <c r="F68" s="14"/>
-      <c r="G68" s="6"/>
-    </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G68" s="14"/>
+      <c r="H68" s="14"/>
+      <c r="I68" s="14"/>
+      <c r="J68" s="14"/>
+      <c r="K68" s="6"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B69" s="5" t="s">
-        <v>215</v>
+        <v>245</v>
       </c>
       <c r="C69" s="14"/>
       <c r="D69" s="14"/>
       <c r="E69" s="14"/>
       <c r="F69" s="14"/>
-      <c r="G69" s="6"/>
-    </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G69" s="14"/>
+      <c r="H69" s="14"/>
+      <c r="I69" s="14"/>
+      <c r="J69" s="14"/>
+      <c r="K69" s="6"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B70" s="5" t="s">
-        <v>216</v>
+        <v>246</v>
       </c>
       <c r="C70" s="14"/>
       <c r="D70" s="14"/>
       <c r="E70" s="14"/>
       <c r="F70" s="14"/>
-      <c r="G70" s="6"/>
-    </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B71" s="5" t="s">
-        <v>217</v>
-      </c>
+      <c r="G70" s="14"/>
+      <c r="H70" s="14"/>
+      <c r="I70" s="14"/>
+      <c r="J70" s="14"/>
+      <c r="K70" s="6"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B71" s="5"/>
       <c r="C71" s="14"/>
       <c r="D71" s="14"/>
       <c r="E71" s="14"/>
       <c r="F71" s="14"/>
-      <c r="G71" s="6"/>
-    </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G71" s="14"/>
+      <c r="H71" s="14"/>
+      <c r="I71" s="14"/>
+      <c r="J71" s="14"/>
+      <c r="K71" s="6"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B72" s="5"/>
       <c r="C72" s="14"/>
       <c r="D72" s="14"/>
       <c r="E72" s="14"/>
       <c r="F72" s="14"/>
-      <c r="G72" s="6"/>
-    </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G72" s="14"/>
+      <c r="H72" s="14"/>
+      <c r="I72" s="14"/>
+      <c r="J72" s="14"/>
+      <c r="K72" s="6"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B73" s="5" t="s">
-        <v>218</v>
+        <v>247</v>
       </c>
       <c r="C73" s="14"/>
       <c r="D73" s="14"/>
       <c r="E73" s="14"/>
       <c r="F73" s="14"/>
-      <c r="G73" s="6"/>
-    </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G73" s="14"/>
+      <c r="H73" s="14"/>
+      <c r="I73" s="14"/>
+      <c r="J73" s="14"/>
+      <c r="K73" s="6"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B74" s="5" t="s">
-        <v>219</v>
+        <v>248</v>
       </c>
       <c r="C74" s="14"/>
       <c r="D74" s="14"/>
       <c r="E74" s="14"/>
       <c r="F74" s="14"/>
-      <c r="G74" s="6"/>
-    </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B75" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="C75" s="8"/>
-      <c r="D75" s="8"/>
-      <c r="E75" s="8"/>
-      <c r="F75" s="8"/>
-      <c r="G75" s="9"/>
+      <c r="G74" s="14"/>
+      <c r="H74" s="14"/>
+      <c r="I74" s="14"/>
+      <c r="J74" s="14"/>
+      <c r="K74" s="6"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B75" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="C75" s="14"/>
+      <c r="D75" s="14"/>
+      <c r="E75" s="14"/>
+      <c r="F75" s="14"/>
+      <c r="G75" s="14"/>
+      <c r="H75" s="14"/>
+      <c r="I75" s="14"/>
+      <c r="J75" s="14"/>
+      <c r="K75" s="6"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B76" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="C76" s="8"/>
+      <c r="D76" s="8"/>
+      <c r="E76" s="8"/>
+      <c r="F76" s="8"/>
+      <c r="G76" s="8"/>
+      <c r="H76" s="8"/>
+      <c r="I76" s="8"/>
+      <c r="J76" s="8"/>
+      <c r="K76" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Inner Apex Class Or Wrapper Class
</commit_message>
<xml_diff>
--- a/me/4.Apex-Classes-and-Methods.xlsx
+++ b/me/4.Apex-Classes-and-Methods.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\salesforce\me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B549528F-53BC-49C0-8E70-003CA62C58F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4171619E-BBD3-4198-97C9-E9771B8DA0FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Apex Class" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="Class Constructor" sheetId="9" r:id="rId9"/>
     <sheet name="Initialization Blocks" sheetId="10" r:id="rId10"/>
     <sheet name="Apex Class Lifecycle" sheetId="11" r:id="rId11"/>
+    <sheet name="InnerApexClassOrWrapperClass" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="344">
   <si>
     <t>Để có overview về các tool khác nhau có thể dùng để viết code Apex trong Salesforce thì thay cho dùng developer console mình sẽ dùng Salesforce set up để tạo class</t>
   </si>
@@ -979,6 +980,157 @@
   </si>
   <si>
     <t>salesforce\4.Apex-Classes-and-Methods\11.apex-class-order-of-execution\dev-console.txt</t>
+  </si>
+  <si>
+    <t>12.inner-class</t>
+  </si>
+  <si>
+    <t>Company.apxc</t>
+  </si>
+  <si>
+    <t>salesforce\4.Apex-Classes-and-Methods\12.inner-class\Company.apxc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * Company Class</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * Stores information about the company</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * and its customers</t>
+  </si>
+  <si>
+    <t>public class Company {</t>
+  </si>
+  <si>
+    <t>public String companyName;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    public String ceo;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    public Integer employeeCount;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    public Long revenue;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    // List of all customers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    private List&lt;Client&gt; customers = new List&lt;Client&gt;();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    // add new customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    public void addNewCustomer(String name, String website, String email, Long phone) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Client customer = new Client(name, website, email, phone);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        customers.add(customer);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    // print the list of all customers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    public void getAllCustomers(){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        for(Client customer : customers){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            System.debug('Customer Name: '+customer.clientName+', Website: '+customer.website+', Phone: '+customer.phone+', Email: '+customer.email);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    // private inner class to store customer information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    private class Client {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        public String clientName;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        public String website;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        public String email;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        public Long phone;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Client (String clientName, String website, String email, Long phone){</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            this.clientName = clientName;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            this.website = website;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            this.email = email;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            this.phone = phone;</t>
+  </si>
+  <si>
+    <t>salesforce\4.Apex-Classes-and-Methods\12.inner-class\dev-console.txt</t>
+  </si>
+  <si>
+    <t>Company sfdcfacts = new Company();</t>
+  </si>
+  <si>
+    <t>sfdcfacts.companyName = 'SFDCFacts Academy';</t>
+  </si>
+  <si>
+    <t>sfdcfacts.ceo = 'Manish Choudhari';</t>
+  </si>
+  <si>
+    <t>sfdcfacts.employeeCount = 6;</t>
+  </si>
+  <si>
+    <t>sfdcfacts.revenue = 1000000;</t>
+  </si>
+  <si>
+    <t>sfdcfacts.addNewCustomer('Forcepanda', 'forcepanda.com', 'forcepanda@gmail.com', 7778889990L);</t>
+  </si>
+  <si>
+    <t>sfdcfacts.addNewCustomer('Udemy', 'udemy.com', 'udemy@gmail.com', 6668889990L);</t>
+  </si>
+  <si>
+    <t>sfdcfacts.getAllCustomers();</t>
+  </si>
+  <si>
+    <r>
+      <t>sfdcfacts.addNewCustomer('CLR Infotech', 'clrinfotech.com', 'clrinfotech@gmail.com', 7778889990</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>inner class Client chỉ được dùng trong class Company</t>
   </si>
 </sst>
 </file>
@@ -2021,6 +2173,417 @@
         <a:xfrm flipH="1">
           <a:off x="3295650" y="19935825"/>
           <a:ext cx="361950" cy="2286000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>56549</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>9043</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A6C5BF0-34BA-E788-63A4-10334793CC60}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="733425" y="533400"/>
+          <a:ext cx="4809524" cy="3857143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>154</xdr:row>
+      <xdr:rowOff>30674</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BB2EA81-414E-5AF1-39D6-40390F77DBAE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="733425" y="24707850"/>
+          <a:ext cx="11287125" cy="4850324"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED93F2AB-95E5-D238-8F31-0FD149BB136D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1724025" y="16335375"/>
+          <a:ext cx="685800" cy="2238375"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C54F8CB-E8D2-01B3-E9C6-A75512F8C25B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1133475" y="18649950"/>
+          <a:ext cx="571500" cy="1047750"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84280521-F761-746C-8298-4494C6E6806B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2152650" y="17687925"/>
+          <a:ext cx="1504950" cy="1057275"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A96906E-2D1B-4480-664B-864A0A753322}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2162175" y="17687925"/>
+          <a:ext cx="3581400" cy="1266825"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE12F2C-24C2-323E-76A2-C2C57A5BA37B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1990725" y="17706975"/>
+          <a:ext cx="5505450" cy="1647825"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Arrow Connector 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{776635C9-FFC2-90D7-96C3-D149DFCB6A79}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4362450" y="19802475"/>
+          <a:ext cx="2028825" cy="3286125"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -5982,7 +6545,7 @@
   <dimension ref="A2:J86"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:H44"/>
+      <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6244,6 +6807,9 @@
       </c>
       <c r="E41" s="10"/>
       <c r="H41" s="6"/>
+      <c r="I41" t="s">
+        <v>5</v>
+      </c>
       <c r="J41" t="s">
         <v>6</v>
       </c>
@@ -6254,6 +6820,9 @@
         <v>125</v>
       </c>
       <c r="H42" s="6"/>
+      <c r="I42" t="s">
+        <v>5</v>
+      </c>
       <c r="J42" t="s">
         <v>6</v>
       </c>
@@ -6264,6 +6833,9 @@
         <v>9</v>
       </c>
       <c r="H43" s="6"/>
+      <c r="I43" t="s">
+        <v>5</v>
+      </c>
       <c r="J43" t="s">
         <v>6</v>
       </c>
@@ -6519,10 +7091,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CDE73B4-8E11-454B-9C53-B6BF2F3BB1B6}">
-  <dimension ref="A2:I105"/>
+  <dimension ref="A2:J105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="J100" sqref="J100"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6729,84 +7301,96 @@
       </c>
       <c r="H32" s="6"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
       <c r="E33" t="s">
         <v>222</v>
       </c>
       <c r="H33" s="6"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
       <c r="D34" t="s">
         <v>251</v>
       </c>
       <c r="H34" s="6"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
       <c r="E35" t="s">
         <v>125</v>
       </c>
       <c r="H35" s="6"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B36" s="5"/>
       <c r="E36" t="s">
         <v>9</v>
       </c>
       <c r="H36" s="6"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B37" s="5"/>
-      <c r="D37" s="13" t="s">
+      <c r="D37" t="s">
         <v>272</v>
       </c>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
       <c r="H37" s="6"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B38" s="5"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13" t="s">
+      <c r="E38" t="s">
         <v>125</v>
       </c>
-      <c r="F38" s="13"/>
       <c r="H38" s="6"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B39" s="5"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13" t="s">
+      <c r="E39" t="s">
         <v>9</v>
       </c>
-      <c r="F39" s="13"/>
       <c r="H39" s="6"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B40" s="5"/>
       <c r="D40" s="10" t="s">
         <v>290</v>
       </c>
       <c r="E40" s="10"/>
       <c r="H40" s="6"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I40" t="s">
+        <v>5</v>
+      </c>
+      <c r="J40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B41" s="5"/>
       <c r="E41" s="10" t="s">
         <v>125</v>
       </c>
       <c r="H41" s="6"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I41" t="s">
+        <v>5</v>
+      </c>
+      <c r="J41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B42" s="5"/>
       <c r="E42" s="10" t="s">
         <v>9</v>
       </c>
       <c r="H42" s="6"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I42" t="s">
+        <v>5</v>
+      </c>
+      <c r="J42" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B43" s="7"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
@@ -6815,12 +7399,12 @@
       <c r="G43" s="8"/>
       <c r="H43" s="9"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
         <v>12</v>
       </c>
@@ -6832,552 +7416,271 @@
       <c r="H47" s="3"/>
       <c r="I47" s="4"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
       <c r="I48" s="6"/>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
       <c r="I49" s="6"/>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
       <c r="I50" s="6"/>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
-      <c r="H51" s="14"/>
       <c r="I51" s="6"/>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
       <c r="I52" s="6"/>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="C53" s="14"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="14"/>
       <c r="I53" s="6"/>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="5"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
-      <c r="H54" s="14"/>
       <c r="I54" s="6"/>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="5"/>
-      <c r="C55" s="14" t="s">
+      <c r="C55" t="s">
         <v>274</v>
       </c>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
       <c r="I55" s="6"/>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="C56" s="14"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14"/>
       <c r="I56" s="6"/>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
       <c r="I57" s="6"/>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C58" s="14"/>
-      <c r="D58" s="14"/>
-      <c r="E58" s="14"/>
-      <c r="F58" s="14"/>
-      <c r="G58" s="14"/>
-      <c r="H58" s="14"/>
       <c r="I58" s="6"/>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" s="5"/>
-      <c r="C59" s="14"/>
-      <c r="D59" s="14"/>
-      <c r="E59" s="14"/>
-      <c r="F59" s="14"/>
-      <c r="G59" s="14"/>
-      <c r="H59" s="14"/>
       <c r="I59" s="6"/>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="C60" s="14"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="14"/>
-      <c r="F60" s="14"/>
-      <c r="G60" s="14"/>
-      <c r="H60" s="14"/>
       <c r="I60" s="6"/>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="C61" s="14"/>
-      <c r="D61" s="14"/>
-      <c r="E61" s="14"/>
-      <c r="F61" s="14"/>
-      <c r="G61" s="14"/>
-      <c r="H61" s="14"/>
       <c r="I61" s="6"/>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="C62" s="14"/>
-      <c r="D62" s="14"/>
-      <c r="E62" s="14"/>
-      <c r="F62" s="14"/>
-      <c r="G62" s="14"/>
-      <c r="H62" s="14"/>
       <c r="I62" s="6"/>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C63" s="14"/>
-      <c r="D63" s="14"/>
-      <c r="E63" s="14"/>
-      <c r="F63" s="14"/>
-      <c r="G63" s="14"/>
-      <c r="H63" s="14"/>
       <c r="I63" s="6"/>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" s="5"/>
-      <c r="C64" s="14"/>
-      <c r="D64" s="14"/>
-      <c r="E64" s="14"/>
-      <c r="F64" s="14"/>
-      <c r="G64" s="14"/>
-      <c r="H64" s="14"/>
       <c r="I64" s="6"/>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" s="5" t="s">
         <v>294</v>
       </c>
-      <c r="C65" s="14"/>
-      <c r="D65" s="14"/>
-      <c r="E65" s="14"/>
-      <c r="F65" s="14"/>
-      <c r="G65" s="14"/>
-      <c r="H65" s="14"/>
       <c r="I65" s="6"/>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="C66" s="14"/>
-      <c r="D66" s="14"/>
-      <c r="E66" s="14"/>
-      <c r="F66" s="14"/>
-      <c r="G66" s="14"/>
-      <c r="H66" s="14"/>
       <c r="I66" s="6"/>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="C67" s="14"/>
-      <c r="D67" s="14"/>
-      <c r="E67" s="14"/>
-      <c r="F67" s="14"/>
-      <c r="G67" s="14"/>
-      <c r="H67" s="14"/>
       <c r="I67" s="6"/>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C68" s="14"/>
-      <c r="D68" s="14"/>
-      <c r="E68" s="14"/>
-      <c r="F68" s="14"/>
-      <c r="G68" s="14"/>
-      <c r="H68" s="14"/>
       <c r="I68" s="6"/>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" s="5"/>
-      <c r="C69" s="14"/>
-      <c r="D69" s="14"/>
-      <c r="E69" s="14"/>
-      <c r="F69" s="14"/>
-      <c r="G69" s="14"/>
-      <c r="H69" s="14"/>
       <c r="I69" s="6"/>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="5" t="s">
         <v>296</v>
       </c>
-      <c r="C70" s="14"/>
-      <c r="D70" s="14"/>
-      <c r="E70" s="14"/>
-      <c r="F70" s="14"/>
-      <c r="G70" s="14"/>
-      <c r="H70" s="14"/>
       <c r="I70" s="6"/>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="C71" s="14"/>
-      <c r="D71" s="14"/>
-      <c r="E71" s="14"/>
-      <c r="F71" s="14"/>
-      <c r="G71" s="14"/>
-      <c r="H71" s="14"/>
       <c r="I71" s="6"/>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="C72" s="14"/>
-      <c r="D72" s="14"/>
-      <c r="E72" s="14"/>
-      <c r="F72" s="14"/>
-      <c r="G72" s="14"/>
-      <c r="H72" s="14"/>
       <c r="I72" s="6"/>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C73" s="14"/>
-      <c r="D73" s="14"/>
-      <c r="E73" s="14"/>
-      <c r="F73" s="14"/>
-      <c r="G73" s="14"/>
-      <c r="H73" s="14"/>
       <c r="I73" s="6"/>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="5"/>
-      <c r="C74" s="14"/>
-      <c r="D74" s="14"/>
-      <c r="E74" s="14"/>
-      <c r="F74" s="14"/>
-      <c r="G74" s="14"/>
-      <c r="H74" s="14"/>
       <c r="I74" s="6"/>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="C75" s="14"/>
-      <c r="D75" s="14"/>
-      <c r="E75" s="14"/>
-      <c r="F75" s="14"/>
-      <c r="G75" s="14"/>
-      <c r="H75" s="14"/>
       <c r="I75" s="6"/>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="C76" s="14"/>
-      <c r="D76" s="14"/>
-      <c r="E76" s="14"/>
-      <c r="F76" s="14"/>
-      <c r="G76" s="14"/>
-      <c r="H76" s="14"/>
       <c r="I76" s="6"/>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="C77" s="14"/>
-      <c r="D77" s="14"/>
-      <c r="E77" s="14"/>
-      <c r="F77" s="14"/>
-      <c r="G77" s="14"/>
-      <c r="H77" s="14"/>
       <c r="I77" s="6"/>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C78" s="14"/>
-      <c r="D78" s="14"/>
-      <c r="E78" s="14"/>
-      <c r="F78" s="14"/>
-      <c r="G78" s="14"/>
-      <c r="H78" s="14"/>
       <c r="I78" s="6"/>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="5"/>
-      <c r="C79" s="14"/>
-      <c r="D79" s="14"/>
-      <c r="E79" s="14"/>
-      <c r="F79" s="14"/>
-      <c r="G79" s="14"/>
-      <c r="H79" s="14"/>
       <c r="I79" s="6"/>
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="C80" s="14"/>
-      <c r="D80" s="14"/>
-      <c r="E80" s="14"/>
-      <c r="F80" s="14"/>
-      <c r="G80" s="14"/>
-      <c r="H80" s="14"/>
       <c r="I80" s="6"/>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="C81" s="14"/>
-      <c r="D81" s="14"/>
-      <c r="E81" s="14"/>
-      <c r="F81" s="14"/>
-      <c r="G81" s="14"/>
-      <c r="H81" s="14"/>
       <c r="I81" s="6"/>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="C82" s="14"/>
-      <c r="D82" s="14"/>
-      <c r="E82" s="14"/>
-      <c r="F82" s="14"/>
-      <c r="G82" s="14"/>
-      <c r="H82" s="14"/>
       <c r="I82" s="6"/>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="C83" s="14"/>
-      <c r="D83" s="14"/>
-      <c r="E83" s="14"/>
-      <c r="F83" s="14"/>
-      <c r="G83" s="14"/>
-      <c r="H83" s="14"/>
       <c r="I83" s="6"/>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="C84" s="14"/>
-      <c r="D84" s="14"/>
-      <c r="E84" s="14"/>
-      <c r="F84" s="14"/>
-      <c r="G84" s="14"/>
-      <c r="H84" s="14"/>
       <c r="I84" s="6"/>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C85" s="14"/>
-      <c r="D85" s="14"/>
-      <c r="E85" s="14"/>
-      <c r="F85" s="14"/>
-      <c r="G85" s="14"/>
-      <c r="H85" s="14"/>
       <c r="I85" s="6"/>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="5"/>
-      <c r="C86" s="14"/>
-      <c r="D86" s="14"/>
-      <c r="E86" s="14"/>
-      <c r="F86" s="14"/>
-      <c r="G86" s="14"/>
-      <c r="H86" s="14"/>
       <c r="I86" s="6"/>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="C87" s="14"/>
-      <c r="D87" s="14"/>
-      <c r="E87" s="14"/>
-      <c r="F87" s="14"/>
-      <c r="G87" s="14"/>
-      <c r="H87" s="14"/>
       <c r="I87" s="6"/>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="C88" s="14"/>
-      <c r="D88" s="14"/>
-      <c r="E88" s="14"/>
-      <c r="F88" s="14"/>
-      <c r="G88" s="14"/>
-      <c r="H88" s="14"/>
       <c r="I88" s="6"/>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="C89" s="14"/>
-      <c r="D89" s="14"/>
-      <c r="E89" s="14"/>
-      <c r="F89" s="14"/>
-      <c r="G89" s="14"/>
-      <c r="H89" s="14"/>
       <c r="I89" s="6"/>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C90" s="14"/>
-      <c r="D90" s="14"/>
-      <c r="E90" s="14"/>
-      <c r="F90" s="14"/>
-      <c r="G90" s="14"/>
-      <c r="H90" s="14"/>
       <c r="I90" s="6"/>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91" s="5"/>
-      <c r="C91" s="14"/>
-      <c r="D91" s="14"/>
-      <c r="E91" s="14"/>
-      <c r="F91" s="14"/>
-      <c r="G91" s="14"/>
-      <c r="H91" s="14"/>
       <c r="I91" s="6"/>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="C92" s="14"/>
-      <c r="D92" s="14"/>
-      <c r="E92" s="14"/>
-      <c r="F92" s="14"/>
-      <c r="G92" s="14"/>
-      <c r="H92" s="14"/>
       <c r="I92" s="6"/>
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B93" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="C93" s="14"/>
-      <c r="D93" s="14"/>
-      <c r="E93" s="14"/>
-      <c r="F93" s="14"/>
-      <c r="G93" s="14"/>
-      <c r="H93" s="14"/>
       <c r="I93" s="6"/>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B94" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C94" s="14"/>
-      <c r="D94" s="14"/>
-      <c r="E94" s="14"/>
-      <c r="F94" s="14"/>
-      <c r="G94" s="14"/>
-      <c r="H94" s="14"/>
       <c r="I94" s="6"/>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.25">
@@ -7410,22 +7713,12 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B100" s="5"/>
-      <c r="C100" s="14"/>
-      <c r="D100" s="14"/>
-      <c r="E100" s="14"/>
-      <c r="F100" s="14"/>
-      <c r="G100" s="14"/>
       <c r="H100" s="6"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B101" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="C101" s="14"/>
-      <c r="D101" s="14"/>
-      <c r="E101" s="14"/>
-      <c r="F101" s="14"/>
-      <c r="G101" s="14"/>
       <c r="H101" s="6"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -7443,6 +7736,1318 @@
       <c r="A105" t="s">
         <v>289</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4F69946-6259-4589-B47D-1310392367DF}">
+  <dimension ref="A26:R127"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D91" workbookViewId="0">
+      <selection activeCell="R105" sqref="R105"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="C28" t="s">
+        <v>3</v>
+      </c>
+      <c r="H28" s="6"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="H29" s="6"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="5"/>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="H30" s="6"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="5"/>
+      <c r="D31" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31" s="6"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
+      <c r="E32" t="s">
+        <v>9</v>
+      </c>
+      <c r="H32" s="6"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="5"/>
+      <c r="E33" t="s">
+        <v>10</v>
+      </c>
+      <c r="H33" s="6"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="5"/>
+      <c r="D34" t="s">
+        <v>31</v>
+      </c>
+      <c r="H34" s="6"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="5"/>
+      <c r="E35" t="s">
+        <v>9</v>
+      </c>
+      <c r="H35" s="6"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="5"/>
+      <c r="E36" t="s">
+        <v>10</v>
+      </c>
+      <c r="H36" s="6"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="5"/>
+      <c r="D37" t="s">
+        <v>48</v>
+      </c>
+      <c r="H37" s="6"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="5"/>
+      <c r="E38" t="s">
+        <v>9</v>
+      </c>
+      <c r="H38" s="6"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="5"/>
+      <c r="E39" t="s">
+        <v>10</v>
+      </c>
+      <c r="H39" s="6"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="5"/>
+      <c r="D40" t="s">
+        <v>102</v>
+      </c>
+      <c r="H40" s="6"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="5"/>
+      <c r="E41" t="s">
+        <v>9</v>
+      </c>
+      <c r="H41" s="6"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="5"/>
+      <c r="E42" t="s">
+        <v>10</v>
+      </c>
+      <c r="H42" s="6"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="5"/>
+      <c r="D43" t="s">
+        <v>124</v>
+      </c>
+      <c r="H43" s="6"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="5"/>
+      <c r="E44" t="s">
+        <v>125</v>
+      </c>
+      <c r="H44" s="6"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="5"/>
+      <c r="E45" t="s">
+        <v>9</v>
+      </c>
+      <c r="H45" s="6"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="5"/>
+      <c r="D46" t="s">
+        <v>161</v>
+      </c>
+      <c r="E46" s="10"/>
+      <c r="H46" s="6"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="5"/>
+      <c r="E47" t="s">
+        <v>162</v>
+      </c>
+      <c r="H47" s="6"/>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48" s="5"/>
+      <c r="D48" t="s">
+        <v>188</v>
+      </c>
+      <c r="H48" s="6"/>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B49" s="5"/>
+      <c r="E49" t="s">
+        <v>9</v>
+      </c>
+      <c r="H49" s="6"/>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B50" s="5"/>
+      <c r="E50" t="s">
+        <v>189</v>
+      </c>
+      <c r="H50" s="6"/>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B51" s="5"/>
+      <c r="D51" t="s">
+        <v>221</v>
+      </c>
+      <c r="H51" s="6"/>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B52" s="5"/>
+      <c r="E52" t="s">
+        <v>9</v>
+      </c>
+      <c r="H52" s="6"/>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B53" s="5"/>
+      <c r="E53" t="s">
+        <v>222</v>
+      </c>
+      <c r="H53" s="6"/>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B54" s="5"/>
+      <c r="D54" t="s">
+        <v>251</v>
+      </c>
+      <c r="H54" s="6"/>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B55" s="5"/>
+      <c r="E55" t="s">
+        <v>125</v>
+      </c>
+      <c r="H55" s="6"/>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B56" s="5"/>
+      <c r="E56" t="s">
+        <v>9</v>
+      </c>
+      <c r="H56" s="6"/>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B57" s="5"/>
+      <c r="D57" t="s">
+        <v>272</v>
+      </c>
+      <c r="H57" s="6"/>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B58" s="5"/>
+      <c r="E58" t="s">
+        <v>125</v>
+      </c>
+      <c r="H58" s="6"/>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B59" s="5"/>
+      <c r="E59" t="s">
+        <v>9</v>
+      </c>
+      <c r="H59" s="6"/>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B60" s="5"/>
+      <c r="D60" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="E60" s="13"/>
+      <c r="F60" s="13"/>
+      <c r="H60" s="6"/>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B61" s="5"/>
+      <c r="D61" s="13"/>
+      <c r="E61" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="F61" s="13"/>
+      <c r="H61" s="6"/>
+    </row>
+    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B62" s="5"/>
+      <c r="D62" s="13"/>
+      <c r="E62" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F62" s="13"/>
+      <c r="H62" s="6"/>
+    </row>
+    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B63" s="5"/>
+      <c r="D63" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="E63" s="10"/>
+      <c r="H63" s="6"/>
+      <c r="I63" t="s">
+        <v>5</v>
+      </c>
+      <c r="J63" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B64" s="5"/>
+      <c r="E64" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="H64" s="6"/>
+      <c r="I64" t="s">
+        <v>5</v>
+      </c>
+      <c r="J64" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B65" s="5"/>
+      <c r="E65" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H65" s="6"/>
+      <c r="I65" t="s">
+        <v>5</v>
+      </c>
+      <c r="J65" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B66" s="7"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="8"/>
+      <c r="E66" s="8"/>
+      <c r="F66" s="8"/>
+      <c r="G66" s="8"/>
+      <c r="H66" s="9"/>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B70" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="3"/>
+      <c r="I70" s="3"/>
+      <c r="J70" s="3"/>
+      <c r="K70" s="3"/>
+      <c r="L70" s="3"/>
+      <c r="M70" s="3"/>
+      <c r="N70" s="3"/>
+      <c r="O70" s="3"/>
+      <c r="P70" s="4"/>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B71" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="C71" s="14"/>
+      <c r="D71" s="14"/>
+      <c r="E71" s="14"/>
+      <c r="F71" s="14"/>
+      <c r="G71" s="14"/>
+      <c r="H71" s="14"/>
+      <c r="I71" s="14"/>
+      <c r="J71" s="14"/>
+      <c r="K71" s="14"/>
+      <c r="L71" s="14"/>
+      <c r="M71" s="14"/>
+      <c r="N71" s="14"/>
+      <c r="O71" s="14"/>
+      <c r="P71" s="6"/>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B72" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="C72" s="14"/>
+      <c r="D72" s="14"/>
+      <c r="E72" s="14"/>
+      <c r="F72" s="14"/>
+      <c r="G72" s="14"/>
+      <c r="H72" s="14"/>
+      <c r="I72" s="14"/>
+      <c r="J72" s="14"/>
+      <c r="K72" s="14"/>
+      <c r="L72" s="14"/>
+      <c r="M72" s="14"/>
+      <c r="N72" s="14"/>
+      <c r="O72" s="14"/>
+      <c r="P72" s="6"/>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B73" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="C73" s="14"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="14"/>
+      <c r="F73" s="14"/>
+      <c r="G73" s="14"/>
+      <c r="H73" s="14"/>
+      <c r="I73" s="14"/>
+      <c r="J73" s="14"/>
+      <c r="K73" s="14"/>
+      <c r="L73" s="14"/>
+      <c r="M73" s="14"/>
+      <c r="N73" s="14"/>
+      <c r="O73" s="14"/>
+      <c r="P73" s="6"/>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B74" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C74" s="14"/>
+      <c r="D74" s="14"/>
+      <c r="E74" s="14"/>
+      <c r="F74" s="14"/>
+      <c r="G74" s="14"/>
+      <c r="H74" s="14"/>
+      <c r="I74" s="14"/>
+      <c r="J74" s="14"/>
+      <c r="K74" s="14"/>
+      <c r="L74" s="14"/>
+      <c r="M74" s="14"/>
+      <c r="N74" s="14"/>
+      <c r="O74" s="14"/>
+      <c r="P74" s="6"/>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B75" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="C75" s="14"/>
+      <c r="D75" s="14"/>
+      <c r="E75" s="14"/>
+      <c r="F75" s="14"/>
+      <c r="G75" s="14"/>
+      <c r="H75" s="14"/>
+      <c r="I75" s="14"/>
+      <c r="J75" s="14"/>
+      <c r="K75" s="14"/>
+      <c r="L75" s="14"/>
+      <c r="M75" s="14"/>
+      <c r="N75" s="14"/>
+      <c r="O75" s="14"/>
+      <c r="P75" s="6"/>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B76" s="5"/>
+      <c r="C76" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="D76" s="14"/>
+      <c r="E76" s="14"/>
+      <c r="F76" s="14"/>
+      <c r="G76" s="14"/>
+      <c r="H76" s="14"/>
+      <c r="I76" s="14"/>
+      <c r="J76" s="14"/>
+      <c r="K76" s="14"/>
+      <c r="L76" s="14"/>
+      <c r="M76" s="14"/>
+      <c r="N76" s="14"/>
+      <c r="O76" s="14"/>
+      <c r="P76" s="6"/>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B77" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="C77" s="14"/>
+      <c r="D77" s="14"/>
+      <c r="E77" s="14"/>
+      <c r="F77" s="14"/>
+      <c r="G77" s="14"/>
+      <c r="H77" s="14"/>
+      <c r="I77" s="14"/>
+      <c r="J77" s="14"/>
+      <c r="K77" s="14"/>
+      <c r="L77" s="14"/>
+      <c r="M77" s="14"/>
+      <c r="N77" s="14"/>
+      <c r="O77" s="14"/>
+      <c r="P77" s="6"/>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B78" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="C78" s="14"/>
+      <c r="D78" s="14"/>
+      <c r="E78" s="14"/>
+      <c r="F78" s="14"/>
+      <c r="G78" s="14"/>
+      <c r="H78" s="14"/>
+      <c r="I78" s="14"/>
+      <c r="J78" s="14"/>
+      <c r="K78" s="14"/>
+      <c r="L78" s="14"/>
+      <c r="M78" s="14"/>
+      <c r="N78" s="14"/>
+      <c r="O78" s="14"/>
+      <c r="P78" s="6"/>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B79" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="C79" s="14"/>
+      <c r="D79" s="14"/>
+      <c r="E79" s="14"/>
+      <c r="F79" s="14"/>
+      <c r="G79" s="14"/>
+      <c r="H79" s="14"/>
+      <c r="I79" s="14"/>
+      <c r="J79" s="14"/>
+      <c r="K79" s="14"/>
+      <c r="L79" s="14"/>
+      <c r="M79" s="14"/>
+      <c r="N79" s="14"/>
+      <c r="O79" s="14"/>
+      <c r="P79" s="6"/>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B80" s="5"/>
+      <c r="C80" s="14"/>
+      <c r="D80" s="14"/>
+      <c r="E80" s="14"/>
+      <c r="F80" s="14"/>
+      <c r="G80" s="14"/>
+      <c r="H80" s="14"/>
+      <c r="I80" s="14"/>
+      <c r="J80" s="14"/>
+      <c r="K80" s="14"/>
+      <c r="L80" s="14"/>
+      <c r="M80" s="14"/>
+      <c r="N80" s="14"/>
+      <c r="O80" s="14"/>
+      <c r="P80" s="6"/>
+    </row>
+    <row r="81" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B81" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="C81" s="14"/>
+      <c r="D81" s="14"/>
+      <c r="E81" s="14"/>
+      <c r="F81" s="14"/>
+      <c r="G81" s="14"/>
+      <c r="H81" s="14"/>
+      <c r="I81" s="14"/>
+      <c r="J81" s="14"/>
+      <c r="K81" s="14"/>
+      <c r="L81" s="14"/>
+      <c r="M81" s="14"/>
+      <c r="N81" s="14"/>
+      <c r="O81" s="14"/>
+      <c r="P81" s="6"/>
+    </row>
+    <row r="82" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B82" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="C82" s="14"/>
+      <c r="D82" s="14"/>
+      <c r="E82" s="14"/>
+      <c r="F82" s="14"/>
+      <c r="G82" s="14"/>
+      <c r="H82" s="14"/>
+      <c r="I82" s="14"/>
+      <c r="J82" s="14"/>
+      <c r="K82" s="14"/>
+      <c r="L82" s="14"/>
+      <c r="M82" s="14"/>
+      <c r="N82" s="14"/>
+      <c r="O82" s="14"/>
+      <c r="P82" s="6"/>
+    </row>
+    <row r="83" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B83" s="5"/>
+      <c r="C83" s="14"/>
+      <c r="D83" s="14"/>
+      <c r="E83" s="14"/>
+      <c r="F83" s="14"/>
+      <c r="G83" s="14"/>
+      <c r="H83" s="14"/>
+      <c r="I83" s="14"/>
+      <c r="J83" s="14"/>
+      <c r="K83" s="14"/>
+      <c r="L83" s="14"/>
+      <c r="M83" s="14"/>
+      <c r="N83" s="14"/>
+      <c r="O83" s="14"/>
+      <c r="P83" s="6"/>
+    </row>
+    <row r="84" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B84" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="C84" s="14"/>
+      <c r="D84" s="14"/>
+      <c r="E84" s="14"/>
+      <c r="F84" s="14"/>
+      <c r="G84" s="14"/>
+      <c r="H84" s="14"/>
+      <c r="I84" s="14"/>
+      <c r="J84" s="14"/>
+      <c r="K84" s="14"/>
+      <c r="L84" s="14"/>
+      <c r="M84" s="14"/>
+      <c r="N84" s="14"/>
+      <c r="O84" s="14"/>
+      <c r="P84" s="6"/>
+    </row>
+    <row r="85" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B85" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="C85" s="14"/>
+      <c r="D85" s="14"/>
+      <c r="E85" s="14"/>
+      <c r="F85" s="14"/>
+      <c r="G85" s="14"/>
+      <c r="H85" s="14"/>
+      <c r="I85" s="14"/>
+      <c r="J85" s="14"/>
+      <c r="K85" s="14"/>
+      <c r="L85" s="14"/>
+      <c r="M85" s="14"/>
+      <c r="N85" s="14"/>
+      <c r="O85" s="14"/>
+      <c r="P85" s="6"/>
+    </row>
+    <row r="86" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B86" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="C86" s="14"/>
+      <c r="D86" s="14"/>
+      <c r="E86" s="14"/>
+      <c r="F86" s="14"/>
+      <c r="G86" s="14"/>
+      <c r="H86" s="14"/>
+      <c r="I86" s="14"/>
+      <c r="J86" s="14"/>
+      <c r="K86" s="14"/>
+      <c r="L86" s="14"/>
+      <c r="M86" s="14"/>
+      <c r="N86" s="14"/>
+      <c r="O86" s="14"/>
+      <c r="P86" s="6"/>
+    </row>
+    <row r="87" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B87" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="C87" s="14"/>
+      <c r="D87" s="14"/>
+      <c r="E87" s="14"/>
+      <c r="F87" s="14"/>
+      <c r="G87" s="14"/>
+      <c r="H87" s="14"/>
+      <c r="I87" s="14"/>
+      <c r="J87" s="14"/>
+      <c r="K87" s="14"/>
+      <c r="L87" s="14"/>
+      <c r="M87" s="14"/>
+      <c r="N87" s="14"/>
+      <c r="O87" s="14"/>
+      <c r="P87" s="6"/>
+    </row>
+    <row r="88" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B88" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C88" s="14"/>
+      <c r="D88" s="14"/>
+      <c r="E88" s="14"/>
+      <c r="F88" s="14"/>
+      <c r="G88" s="14"/>
+      <c r="H88" s="14"/>
+      <c r="I88" s="14"/>
+      <c r="J88" s="14"/>
+      <c r="K88" s="14"/>
+      <c r="L88" s="14"/>
+      <c r="M88" s="14"/>
+      <c r="N88" s="14"/>
+      <c r="O88" s="14"/>
+      <c r="P88" s="6"/>
+    </row>
+    <row r="89" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B89" s="5"/>
+      <c r="C89" s="14"/>
+      <c r="D89" s="14"/>
+      <c r="E89" s="14"/>
+      <c r="F89" s="14"/>
+      <c r="G89" s="14"/>
+      <c r="H89" s="14"/>
+      <c r="I89" s="14"/>
+      <c r="J89" s="14"/>
+      <c r="K89" s="14"/>
+      <c r="L89" s="14"/>
+      <c r="M89" s="14"/>
+      <c r="N89" s="14"/>
+      <c r="O89" s="14"/>
+      <c r="P89" s="6"/>
+    </row>
+    <row r="90" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B90" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C90" s="14"/>
+      <c r="D90" s="14"/>
+      <c r="E90" s="14"/>
+      <c r="F90" s="14"/>
+      <c r="G90" s="14"/>
+      <c r="H90" s="14"/>
+      <c r="I90" s="14"/>
+      <c r="J90" s="14"/>
+      <c r="K90" s="14"/>
+      <c r="L90" s="14"/>
+      <c r="M90" s="14"/>
+      <c r="N90" s="14"/>
+      <c r="O90" s="14"/>
+      <c r="P90" s="6"/>
+    </row>
+    <row r="91" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B91" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="C91" s="14"/>
+      <c r="D91" s="14"/>
+      <c r="E91" s="14"/>
+      <c r="F91" s="14"/>
+      <c r="G91" s="14"/>
+      <c r="H91" s="14"/>
+      <c r="I91" s="14"/>
+      <c r="J91" s="14"/>
+      <c r="K91" s="14"/>
+      <c r="L91" s="14"/>
+      <c r="M91" s="14"/>
+      <c r="N91" s="14"/>
+      <c r="O91" s="14"/>
+      <c r="P91" s="6"/>
+    </row>
+    <row r="92" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B92" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="C92" s="14"/>
+      <c r="D92" s="14"/>
+      <c r="E92" s="14"/>
+      <c r="F92" s="14"/>
+      <c r="G92" s="14"/>
+      <c r="H92" s="14"/>
+      <c r="I92" s="14"/>
+      <c r="J92" s="14"/>
+      <c r="K92" s="14"/>
+      <c r="L92" s="14"/>
+      <c r="M92" s="14"/>
+      <c r="N92" s="14"/>
+      <c r="O92" s="14"/>
+      <c r="P92" s="6"/>
+    </row>
+    <row r="93" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B93" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="C93" s="14"/>
+      <c r="D93" s="14"/>
+      <c r="E93" s="14"/>
+      <c r="F93" s="14"/>
+      <c r="G93" s="14"/>
+      <c r="H93" s="14"/>
+      <c r="I93" s="14"/>
+      <c r="J93" s="14"/>
+      <c r="K93" s="14"/>
+      <c r="L93" s="14"/>
+      <c r="M93" s="14"/>
+      <c r="N93" s="14"/>
+      <c r="O93" s="14"/>
+      <c r="P93" s="6"/>
+    </row>
+    <row r="94" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B94" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C94" s="14"/>
+      <c r="D94" s="14"/>
+      <c r="E94" s="14"/>
+      <c r="F94" s="14"/>
+      <c r="G94" s="14"/>
+      <c r="H94" s="14"/>
+      <c r="I94" s="14"/>
+      <c r="J94" s="14"/>
+      <c r="K94" s="14"/>
+      <c r="L94" s="14"/>
+      <c r="M94" s="14"/>
+      <c r="N94" s="14"/>
+      <c r="O94" s="14"/>
+      <c r="P94" s="6"/>
+    </row>
+    <row r="95" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B95" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C95" s="14"/>
+      <c r="D95" s="14"/>
+      <c r="E95" s="14"/>
+      <c r="F95" s="14"/>
+      <c r="G95" s="14"/>
+      <c r="H95" s="14"/>
+      <c r="I95" s="14"/>
+      <c r="J95" s="14"/>
+      <c r="K95" s="14"/>
+      <c r="L95" s="14"/>
+      <c r="M95" s="14"/>
+      <c r="N95" s="14"/>
+      <c r="O95" s="14"/>
+      <c r="P95" s="6"/>
+    </row>
+    <row r="96" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B96" s="5"/>
+      <c r="C96" s="14"/>
+      <c r="D96" s="14"/>
+      <c r="E96" s="14"/>
+      <c r="F96" s="14"/>
+      <c r="G96" s="14"/>
+      <c r="H96" s="14"/>
+      <c r="I96" s="14"/>
+      <c r="J96" s="14"/>
+      <c r="K96" s="14"/>
+      <c r="L96" s="14"/>
+      <c r="M96" s="14"/>
+      <c r="N96" s="14"/>
+      <c r="O96" s="14"/>
+      <c r="P96" s="6"/>
+    </row>
+    <row r="97" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B97" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="C97" s="14"/>
+      <c r="D97" s="14"/>
+      <c r="E97" s="14"/>
+      <c r="F97" s="14"/>
+      <c r="G97" s="14"/>
+      <c r="H97" s="14"/>
+      <c r="I97" s="14"/>
+      <c r="J97" s="14"/>
+      <c r="K97" s="14"/>
+      <c r="L97" s="14"/>
+      <c r="M97" s="14"/>
+      <c r="N97" s="14"/>
+      <c r="O97" s="14"/>
+      <c r="P97" s="6"/>
+    </row>
+    <row r="98" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B98" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="C98" s="14"/>
+      <c r="D98" s="14"/>
+      <c r="E98" s="14"/>
+      <c r="F98" s="14"/>
+      <c r="G98" s="14"/>
+      <c r="H98" s="14"/>
+      <c r="I98" s="14"/>
+      <c r="J98" s="14"/>
+      <c r="K98" s="14"/>
+      <c r="L98" s="14"/>
+      <c r="M98" s="14"/>
+      <c r="N98" s="14"/>
+      <c r="O98" s="14"/>
+      <c r="P98" s="6"/>
+    </row>
+    <row r="99" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B99" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="C99" s="14"/>
+      <c r="D99" s="14"/>
+      <c r="E99" s="14"/>
+      <c r="F99" s="14"/>
+      <c r="G99" s="14"/>
+      <c r="H99" s="14"/>
+      <c r="I99" s="14"/>
+      <c r="J99" s="14"/>
+      <c r="K99" s="14"/>
+      <c r="L99" s="14"/>
+      <c r="M99" s="14"/>
+      <c r="N99" s="14"/>
+      <c r="O99" s="14"/>
+      <c r="P99" s="6"/>
+    </row>
+    <row r="100" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B100" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="C100" s="14"/>
+      <c r="D100" s="14"/>
+      <c r="E100" s="14"/>
+      <c r="F100" s="14"/>
+      <c r="G100" s="14"/>
+      <c r="H100" s="14"/>
+      <c r="I100" s="14"/>
+      <c r="J100" s="14"/>
+      <c r="K100" s="14"/>
+      <c r="L100" s="14"/>
+      <c r="M100" s="14"/>
+      <c r="N100" s="14"/>
+      <c r="O100" s="14"/>
+      <c r="P100" s="6"/>
+    </row>
+    <row r="101" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B101" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="C101" s="14"/>
+      <c r="D101" s="14"/>
+      <c r="E101" s="14"/>
+      <c r="F101" s="14"/>
+      <c r="G101" s="14"/>
+      <c r="H101" s="14"/>
+      <c r="I101" s="14"/>
+      <c r="J101" s="14"/>
+      <c r="K101" s="14"/>
+      <c r="L101" s="14"/>
+      <c r="M101" s="14"/>
+      <c r="N101" s="14"/>
+      <c r="O101" s="14"/>
+      <c r="P101" s="6"/>
+    </row>
+    <row r="102" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B102" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="C102" s="14"/>
+      <c r="D102" s="14"/>
+      <c r="E102" s="14"/>
+      <c r="F102" s="14"/>
+      <c r="G102" s="14"/>
+      <c r="H102" s="14"/>
+      <c r="I102" s="14"/>
+      <c r="J102" s="14"/>
+      <c r="K102" s="14"/>
+      <c r="L102" s="14"/>
+      <c r="M102" s="14"/>
+      <c r="N102" s="14"/>
+      <c r="O102" s="14"/>
+      <c r="P102" s="6"/>
+    </row>
+    <row r="103" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B103" s="5"/>
+      <c r="C103" s="14"/>
+      <c r="D103" s="14"/>
+      <c r="E103" s="14"/>
+      <c r="F103" s="14"/>
+      <c r="G103" s="14"/>
+      <c r="H103" s="14"/>
+      <c r="I103" s="14"/>
+      <c r="J103" s="14"/>
+      <c r="K103" s="14"/>
+      <c r="L103" s="14"/>
+      <c r="M103" s="14"/>
+      <c r="N103" s="14"/>
+      <c r="O103" s="14"/>
+      <c r="P103" s="6"/>
+    </row>
+    <row r="104" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B104" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="C104" s="14"/>
+      <c r="D104" s="14"/>
+      <c r="E104" s="14"/>
+      <c r="F104" s="14"/>
+      <c r="G104" s="14"/>
+      <c r="H104" s="14"/>
+      <c r="I104" s="14"/>
+      <c r="J104" s="14"/>
+      <c r="K104" s="14"/>
+      <c r="L104" s="14"/>
+      <c r="M104" s="14"/>
+      <c r="N104" s="14"/>
+      <c r="O104" s="14"/>
+      <c r="P104" s="6"/>
+      <c r="Q104" t="s">
+        <v>5</v>
+      </c>
+      <c r="R104" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="105" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B105" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="C105" s="14"/>
+      <c r="D105" s="14"/>
+      <c r="E105" s="14"/>
+      <c r="F105" s="14"/>
+      <c r="G105" s="14"/>
+      <c r="H105" s="14"/>
+      <c r="I105" s="14"/>
+      <c r="J105" s="14"/>
+      <c r="K105" s="14"/>
+      <c r="L105" s="14"/>
+      <c r="M105" s="14"/>
+      <c r="N105" s="14"/>
+      <c r="O105" s="14"/>
+      <c r="P105" s="6"/>
+    </row>
+    <row r="106" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B106" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="C106" s="14"/>
+      <c r="D106" s="14"/>
+      <c r="E106" s="14"/>
+      <c r="F106" s="14"/>
+      <c r="G106" s="14"/>
+      <c r="H106" s="14"/>
+      <c r="I106" s="14"/>
+      <c r="J106" s="14"/>
+      <c r="K106" s="14"/>
+      <c r="L106" s="14"/>
+      <c r="M106" s="14"/>
+      <c r="N106" s="14"/>
+      <c r="O106" s="14"/>
+      <c r="P106" s="6"/>
+    </row>
+    <row r="107" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B107" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="C107" s="14"/>
+      <c r="D107" s="14"/>
+      <c r="E107" s="14"/>
+      <c r="F107" s="14"/>
+      <c r="G107" s="14"/>
+      <c r="H107" s="14"/>
+      <c r="I107" s="14"/>
+      <c r="J107" s="14"/>
+      <c r="K107" s="14"/>
+      <c r="L107" s="14"/>
+      <c r="M107" s="14"/>
+      <c r="N107" s="14"/>
+      <c r="O107" s="14"/>
+      <c r="P107" s="6"/>
+    </row>
+    <row r="108" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B108" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="C108" s="14"/>
+      <c r="D108" s="14"/>
+      <c r="E108" s="14"/>
+      <c r="F108" s="14"/>
+      <c r="G108" s="14"/>
+      <c r="H108" s="14"/>
+      <c r="I108" s="14"/>
+      <c r="J108" s="14"/>
+      <c r="K108" s="14"/>
+      <c r="L108" s="14"/>
+      <c r="M108" s="14"/>
+      <c r="N108" s="14"/>
+      <c r="O108" s="14"/>
+      <c r="P108" s="6"/>
+    </row>
+    <row r="109" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B109" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C109" s="14"/>
+      <c r="D109" s="14"/>
+      <c r="E109" s="14"/>
+      <c r="F109" s="14"/>
+      <c r="G109" s="14"/>
+      <c r="H109" s="14"/>
+      <c r="I109" s="14"/>
+      <c r="J109" s="14"/>
+      <c r="K109" s="14"/>
+      <c r="L109" s="14"/>
+      <c r="M109" s="14"/>
+      <c r="N109" s="14"/>
+      <c r="O109" s="14"/>
+      <c r="P109" s="6"/>
+    </row>
+    <row r="110" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B110" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C110" s="14"/>
+      <c r="D110" s="14"/>
+      <c r="E110" s="14"/>
+      <c r="F110" s="14"/>
+      <c r="G110" s="14"/>
+      <c r="H110" s="14"/>
+      <c r="I110" s="14"/>
+      <c r="J110" s="14"/>
+      <c r="K110" s="14"/>
+      <c r="L110" s="14"/>
+      <c r="M110" s="14"/>
+      <c r="N110" s="14"/>
+      <c r="O110" s="14"/>
+      <c r="P110" s="6"/>
+    </row>
+    <row r="111" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B111" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C111" s="8"/>
+      <c r="D111" s="8"/>
+      <c r="E111" s="8"/>
+      <c r="F111" s="8"/>
+      <c r="G111" s="8"/>
+      <c r="H111" s="8"/>
+      <c r="I111" s="8"/>
+      <c r="J111" s="8"/>
+      <c r="K111" s="8"/>
+      <c r="L111" s="8"/>
+      <c r="M111" s="8"/>
+      <c r="N111" s="8"/>
+      <c r="O111" s="8"/>
+      <c r="P111" s="9"/>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B115" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="C115" s="3"/>
+      <c r="D115" s="3"/>
+      <c r="E115" s="3"/>
+      <c r="F115" s="3"/>
+      <c r="G115" s="3"/>
+      <c r="H115" s="3"/>
+      <c r="I115" s="3"/>
+      <c r="J115" s="3"/>
+      <c r="K115" s="4"/>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B116" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="C116" s="14"/>
+      <c r="D116" s="14"/>
+      <c r="E116" s="14"/>
+      <c r="F116" s="14"/>
+      <c r="G116" s="14"/>
+      <c r="H116" s="14"/>
+      <c r="I116" s="14"/>
+      <c r="J116" s="14"/>
+      <c r="K116" s="6"/>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B117" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="C117" s="14"/>
+      <c r="D117" s="14"/>
+      <c r="E117" s="14"/>
+      <c r="F117" s="14"/>
+      <c r="G117" s="14"/>
+      <c r="H117" s="14"/>
+      <c r="I117" s="14"/>
+      <c r="J117" s="14"/>
+      <c r="K117" s="6"/>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B118" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="C118" s="14"/>
+      <c r="D118" s="14"/>
+      <c r="E118" s="14"/>
+      <c r="F118" s="14"/>
+      <c r="G118" s="14"/>
+      <c r="H118" s="14"/>
+      <c r="I118" s="14"/>
+      <c r="J118" s="14"/>
+      <c r="K118" s="6"/>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B119" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="C119" s="14"/>
+      <c r="D119" s="14"/>
+      <c r="E119" s="14"/>
+      <c r="F119" s="14"/>
+      <c r="G119" s="14"/>
+      <c r="H119" s="14"/>
+      <c r="I119" s="14"/>
+      <c r="J119" s="14"/>
+      <c r="K119" s="6"/>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B120" s="5"/>
+      <c r="C120" s="14"/>
+      <c r="D120" s="14"/>
+      <c r="E120" s="14"/>
+      <c r="F120" s="14"/>
+      <c r="G120" s="14"/>
+      <c r="H120" s="14"/>
+      <c r="I120" s="14"/>
+      <c r="J120" s="14"/>
+      <c r="K120" s="6"/>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B121" s="5"/>
+      <c r="C121" s="14"/>
+      <c r="D121" s="14"/>
+      <c r="E121" s="14"/>
+      <c r="F121" s="14"/>
+      <c r="G121" s="14"/>
+      <c r="H121" s="14"/>
+      <c r="I121" s="14"/>
+      <c r="J121" s="14"/>
+      <c r="K121" s="6"/>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B122" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="C122" s="14"/>
+      <c r="D122" s="14"/>
+      <c r="E122" s="14"/>
+      <c r="F122" s="14"/>
+      <c r="G122" s="14"/>
+      <c r="H122" s="14"/>
+      <c r="I122" s="14"/>
+      <c r="J122" s="14"/>
+      <c r="K122" s="6"/>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B123" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="C123" s="14"/>
+      <c r="D123" s="14"/>
+      <c r="E123" s="14"/>
+      <c r="F123" s="14"/>
+      <c r="G123" s="14"/>
+      <c r="H123" s="14"/>
+      <c r="I123" s="14"/>
+      <c r="J123" s="14"/>
+      <c r="K123" s="6"/>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B124" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="C124" s="14"/>
+      <c r="D124" s="14"/>
+      <c r="E124" s="14"/>
+      <c r="F124" s="14"/>
+      <c r="G124" s="14"/>
+      <c r="H124" s="14"/>
+      <c r="I124" s="14"/>
+      <c r="J124" s="14"/>
+      <c r="K124" s="6"/>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B125" s="5"/>
+      <c r="C125" s="14"/>
+      <c r="D125" s="14"/>
+      <c r="E125" s="14"/>
+      <c r="F125" s="14"/>
+      <c r="G125" s="14"/>
+      <c r="H125" s="14"/>
+      <c r="I125" s="14"/>
+      <c r="J125" s="14"/>
+      <c r="K125" s="6"/>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B126" s="5"/>
+      <c r="C126" s="14"/>
+      <c r="D126" s="14"/>
+      <c r="E126" s="14"/>
+      <c r="F126" s="14"/>
+      <c r="G126" s="14"/>
+      <c r="H126" s="14"/>
+      <c r="I126" s="14"/>
+      <c r="J126" s="14"/>
+      <c r="K126" s="6"/>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B127" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="C127" s="8"/>
+      <c r="D127" s="8"/>
+      <c r="E127" s="8"/>
+      <c r="F127" s="8"/>
+      <c r="G127" s="8"/>
+      <c r="H127" s="8"/>
+      <c r="I127" s="8"/>
+      <c r="J127" s="8"/>
+      <c r="K127" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>